<commit_message>
Added real planning + technical documentation V0.3 +  update logbook
</commit_message>
<xml_diff>
--- a/JournalDeBords.xlsx
+++ b/JournalDeBords.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="65" documentId="13_ncr:1_{581317AF-9E9B-48A5-9EDF-E0687D23730A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{B4E352CC-02EF-438A-8BAD-60A821B65B71}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E675FB9-10CD-43EE-A7E4-0C8EBD63A034}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,69 +20,111 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>Documentation</t>
   </si>
   <si>
+    <t>Backlog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transformation des </t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Heure</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Mail Planification</t>
+  </si>
+  <si>
+    <t>Lecture de l'énoncé</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> création de V 0.1 passage de V0.1 aV0.2</t>
+  </si>
+  <si>
+    <t>Création GitHub</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> réponse Q1</t>
+  </si>
+  <si>
+    <t>Modification de la planification initial</t>
+  </si>
+  <si>
+    <t>MLD</t>
+  </si>
+  <si>
+    <t>Planification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planification </t>
+  </si>
+  <si>
+    <t>Q6</t>
+  </si>
+  <si>
+    <t>Contact avec Responsable TPI</t>
+  </si>
+  <si>
+    <t>Creation données</t>
+  </si>
+  <si>
+    <t>Mail à Responsable TPI</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Implémentation BD</t>
+  </si>
+  <si>
+    <t>Creation BD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aide par Clément Christensen </t>
+  </si>
+  <si>
+    <t>pour sécuriser le dossier model</t>
+  </si>
+  <si>
+    <t>Réponse Q4</t>
+  </si>
+  <si>
     <t>RDV avec Responsable TPI</t>
   </si>
   <si>
-    <t>Backlog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transformation des </t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>Q3</t>
-  </si>
-  <si>
-    <t>Q4</t>
-  </si>
-  <si>
-    <t>Q5</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Heure</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Mail Planification</t>
-  </si>
-  <si>
-    <t>Planification (GANT)</t>
-  </si>
-  <si>
-    <t>Lecture de l'énoncé</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> création de V 0.1 passage de V0.1 aV0.2</t>
-  </si>
-  <si>
-    <t>Création GitHub</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> réponse Q1</t>
-  </si>
-  <si>
-    <t>Modification de la planification initial</t>
-  </si>
-  <si>
-    <t>Réponse Q5</t>
+    <t>V0.2 a V0.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> réponse Q2,Q3,Q5,Q6</t>
+  </si>
+  <si>
+    <t>Plaification Effectif</t>
   </si>
 </sst>
 </file>
@@ -154,8 +196,8 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>46545</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="9" name="Encre 8">
@@ -174,7 +216,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="9" name="Encre 8">
@@ -504,31 +546,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.53125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -539,12 +581,12 @@
         <v>0.3125</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -552,7 +594,7 @@
         <v>0.3263888888888889</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -563,7 +605,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -571,7 +613,7 @@
         <v>0.4548611111111111</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
@@ -579,10 +621,10 @@
         <v>0.46527777777777773</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
@@ -590,10 +632,10 @@
         <v>0.47222222222222227</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
@@ -601,73 +643,184 @@
         <v>0.52777777777777779</v>
       </c>
       <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
         <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B12" s="2">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B13" s="2">
-        <v>0.59027777777777779</v>
-      </c>
-      <c r="C13" t="s">
-        <v>0</v>
-      </c>
-    </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B14" s="2">
+        <v>0.66319444444444442</v>
+      </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B15" s="2">
-        <v>0.66319444444444442</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B16" s="2">
+        <v>0.68402777777777779</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B17" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" s="1">
+        <v>43558</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B19" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B21" s="2">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B22" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B23" s="2">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B24" s="2">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B25" s="2">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B26" s="2"/>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B28" s="2">
+        <v>0.59375</v>
+      </c>
+      <c r="C28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B29" s="2">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="C29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B30" s="2">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B17" s="2">
-        <v>0.68402777777777779</v>
-      </c>
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B18" s="2">
-        <v>0.6875</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="C30" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B31" s="2">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>